<commit_message>
update resume and applied jobs
also, down with the typos!
</commit_message>
<xml_diff>
--- a/work_experience/data/applied jobs.xlsx
+++ b/work_experience/data/applied jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\einel\Documents\Projects\einelson.github.io\work_experience\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7544CFB6-8816-42AB-8880-5635C107D6FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6DF27F-3664-4372-B612-20340CF61E18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
   <si>
     <t>Applied</t>
   </si>
@@ -141,15 +141,9 @@
     <t>Software intern</t>
   </si>
   <si>
-    <t>Concact form</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Contact orm</t>
-  </si>
-  <si>
     <t>Study up on UDP, TCP, OSI levels. Ham radio</t>
   </si>
   <si>
@@ -331,6 +325,12 @@
   </si>
   <si>
     <t>Florida</t>
+  </si>
+  <si>
+    <t>Radio wave, ham radio</t>
+  </si>
+  <si>
+    <t>Contact form</t>
   </si>
 </sst>
 </file>
@@ -667,22 +667,22 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.40625" customWidth="1"/>
-    <col min="3" max="3" width="34.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.40625" customWidth="1"/>
-    <col min="5" max="5" width="10.40625" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="1" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -708,10 +708,10 @@
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -722,13 +722,13 @@
         <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -739,13 +739,13 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -753,13 +753,13 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -767,13 +767,13 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -787,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -795,7 +795,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -804,7 +804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -812,7 +812,7 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -821,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -829,13 +829,13 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -843,13 +843,13 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -857,10 +857,10 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -869,10 +869,10 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -880,16 +880,16 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -897,7 +897,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -906,10 +906,10 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -917,30 +917,30 @@
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -960,10 +960,10 @@
         <v>35</v>
       </c>
       <c r="I16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.75">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -971,348 +971,363 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A25" t="s">
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A26" t="s">
+      <c r="D26" t="s">
         <v>58</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
-      <c r="D26" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>60</v>
       </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A27" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A28" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A29" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A31" t="s">
+      <c r="D31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>66</v>
       </c>
-      <c r="D31" t="s">
+      <c r="B32" t="s">
         <v>67</v>
       </c>
-      <c r="E31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>69</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>70</v>
       </c>
-      <c r="D32" t="s">
+      <c r="B34" t="s">
         <v>67</v>
       </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A33" t="s">
+      <c r="C34" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A34" t="s">
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>72</v>
       </c>
-      <c r="B34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>73</v>
       </c>
-      <c r="D34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
         <v>75</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>76</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>77</v>
       </c>
-      <c r="D36" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A37" t="s">
+      <c r="B38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
         <v>78</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A38" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D40" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A40" t="s">
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
         <v>89</v>
       </c>
-      <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A41" t="s">
+      <c r="D42" t="s">
         <v>90</v>
       </c>
-      <c r="B41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A42" t="s">
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
         <v>93</v>
       </c>
-      <c r="B42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" t="s">
-        <v>92</v>
-      </c>
-      <c r="E42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A43" t="s">
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>94</v>
       </c>
-      <c r="B43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" t="s">
         <v>95</v>
-      </c>
-      <c r="D43" t="s">
-        <v>88</v>
-      </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A44" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" t="s">
-        <v>66</v>
-      </c>
-      <c r="D44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.75">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
-        <v>100</v>
-      </c>
-      <c r="E45" t="s">
-        <v>12</v>
-      </c>
-      <c r="I45" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>